<commit_message>
update schedule for 2024
</commit_message>
<xml_diff>
--- a/ids720_specific/class_schedule_xlsx.xlsx
+++ b/ids720_specific/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids720_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39265EB0-12CC-D046-82DD-3CD625E45E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531FE134-F74D-9743-8D35-63A3D9ED9AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3120" yWindow="760" windowWidth="26820" windowHeight="17640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Topic</t>
   </si>
@@ -102,9 +102,6 @@
 - Regex</t>
   </si>
   <si>
-    <t>THANKSGIVING</t>
-  </si>
-  <si>
     <t>- Class Introduction
 - Welcome to VS Code</t>
   </si>
@@ -129,9 +126,6 @@
   <si>
     <t>- Defensive Programming
 - Groupby / Split-Apply-Combine</t>
-  </si>
-  <si>
-    <t>**Final Project Report and Presentation Due**</t>
   </si>
   <si>
     <t>- JVP Chapter 5 up to "Hyperparameters and Model Validation" Section (pp 331 - 359)</t>
@@ -145,9 +139,6 @@
 - `Patsy: Differences from R &lt;https://patsy.readthedocs.io/en/latest/R-comparison.html&gt;`_</t>
   </si>
   <si>
-    <t>No Class</t>
-  </si>
-  <si>
     <t>- **SETUP 1:** `Installing Python and miniconda &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_python.html&gt;`_
 - **SETUP 2:** `Installing and Configuring VS Code &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_vscode.html&gt;`_
 - `chatGPT and You &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/99_advice/llms.html&gt;`_</t>
@@ -168,94 +159,7 @@
 - `Python v. R &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/python_v_r.html&gt;`_</t>
   </si>
   <si>
-    <t>Tues, Aug 29</t>
-  </si>
-  <si>
-    <t>Thurs, Aug 31</t>
-  </si>
-  <si>
-    <t>Fri, Sep 1</t>
-  </si>
-  <si>
-    <t>Tues, Sep 5</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 7</t>
-  </si>
-  <si>
-    <t>Tues, Sep 12</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 14</t>
-  </si>
-  <si>
-    <t>Tues, Sep 19</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 21</t>
-  </si>
-  <si>
-    <t>Tues, Sep 26</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 28</t>
-  </si>
-  <si>
-    <t>Tues, Oct 3</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 5</t>
-  </si>
-  <si>
     <t>**FALL BREAK**</t>
-  </si>
-  <si>
-    <t>Tues, Oct 10</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 12</t>
-  </si>
-  <si>
-    <t>Tues, Oct 17</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 19</t>
-  </si>
-  <si>
-    <t>Tues, Oct 24</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 26</t>
-  </si>
-  <si>
-    <t>Tues, Oct 31</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 2</t>
-  </si>
-  <si>
-    <t>Tues, Nov 7</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 9</t>
-  </si>
-  <si>
-    <t>Tues, Nov 14</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 16</t>
-  </si>
-  <si>
-    <t>Tues, Nov 21</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 23</t>
-  </si>
-  <si>
-    <t>Tues, Nov 28</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 30</t>
   </si>
   <si>
     <t>- `Advanced Command Line &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/10_commandline/commandline_part2.html&gt;`_
@@ -345,9 +249,6 @@
     <t>- `Link &lt;exercises/Exercise_merging.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Wed Dec 13</t>
-  </si>
-  <si>
     <t>- `Plotting in Python through seaborn and Grammer of Graphics &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/class_5/week_2/10_plotting_in_python.html&gt;`_</t>
   </si>
   <si>
@@ -372,9 +273,6 @@
 - `Strategies for Big Data &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/30_big_data/20_big_data_strategies.html&gt;`_
 - Download the dataset linked at the top of the linked exercise before class.
 - `Parquet Format &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/30_big_data/30_parquet.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Ex &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Workflow Management &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/workflow.html&gt;`_
@@ -426,13 +324,109 @@
 - **Opioid Project Rough Draft Due**</t>
   </si>
   <si>
-    <t>- `Link &lt;execises/Exercise_codeyourownlinearregression.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>Catchup Time</t>
+    <t>Tues, Aug 27</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 29</t>
+  </si>
+  <si>
+    <t>Fri, Aug 30</t>
+  </si>
+  <si>
+    <t>Tues, Sep 3</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 5</t>
+  </si>
+  <si>
+    <t>Tues, Sep 10</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 12</t>
+  </si>
+  <si>
+    <t>Tues, Sep 17</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 19</t>
+  </si>
+  <si>
+    <t>Tues, Sep 24</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 26</t>
+  </si>
+  <si>
+    <t>Tues, Oct 1</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 3</t>
+  </si>
+  <si>
+    <t>Tues, Oct 8</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 10</t>
+  </si>
+  <si>
+    <t>Tues, Oct 15</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 17</t>
+  </si>
+  <si>
+    <t>Tues, Oct 22</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 24</t>
+  </si>
+  <si>
+    <t>Tues, Oct 29</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 31</t>
+  </si>
+  <si>
+    <t>Tues, Nov 5</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 7</t>
+  </si>
+  <si>
+    <t>Tues, Nov 12</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 14</t>
+  </si>
+  <si>
+    <t>Tues, Nov 19</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 21</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>**Discuss mid-semester project in class**</t>
+  </si>
+  <si>
+    <t>[finish groupby and reshaping exercises]</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/Exercise_codeyourownlinearregression.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>**FALL BREAK** (Not technically, but take the week)</t>
+  </si>
+  <si>
+    <t>LAST CLASS</t>
+  </si>
+  <si>
+    <t>**Final Project Report Due**</t>
+  </si>
+  <si>
+    <t>Wed Dec 12</t>
   </si>
 </sst>
 </file>
@@ -539,9 +533,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -579,7 +573,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -685,7 +679,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -827,7 +821,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -835,15 +829,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="105.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="57.1640625" customWidth="1"/>
@@ -865,33 +859,33 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -902,83 +896,83 @@
     </row>
     <row r="5" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="165" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>16</v>
@@ -986,257 +980,241 @@
     </row>
     <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>48</v>
+        <v>83</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="71" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>98</v>
+        <v>61</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="135" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
+        <v>94</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readings for Thursday
</commit_message>
<xml_diff>
--- a/ids720_specific/class_schedule_xlsx.xlsx
+++ b/ids720_specific/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids720_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB3BA3C-A825-EE43-A497-602B5FC11CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB4B8B4-34AF-3841-9961-5B333D57EA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -238,9 +238,6 @@
 </t>
   </si>
   <si>
-    <t>- `Data Manipulations, Concatenating and Merging (NOT grouping or querying subsections on left navigation) &lt;../notebooks/class_3/week_4/00_intro_to_querying_data.html&gt;`_</t>
-  </si>
-  <si>
     <t>- `What is Big Data? &lt;../notebooks/PDS_not_yet_in_coursera/30_big_data/10_big_data_what_is_it.html&gt;`_
 - `Strategies for Big Data &lt;../notebooks/PDS_not_yet_in_coursera/30_big_data/20_big_data_strategies.html&gt;`_
 - Download the dataset linked at the top of the linked exercise before class.
@@ -432,6 +429,11 @@
 - `Making Pretty Plots 1 &lt;../notebooks/class_5/week_1/2.2.1_making_plots_pretty_1.html&gt;`_
 - `Making Pretty Plots 2 &lt;../notebooks/class_5/week_1/2.2.2_making_plots_pretty_2.html&gt;`_
 - `Pandas Plotting &lt;../notebooks/class_5/week_1/1.6.1_plotting_with_pandas.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Combining, Grouping and Querying &lt;../notebooks/class_3/week_4/00_intro_to_querying_data.html&gt;`_
+- `Concatenating &lt;../notebooks/class_3/week_4/10_combining_concatenating.html&gt;`_
+- `Merging/Joins &lt;../notebooks/class_3/week_4/15_combining_merging.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -840,7 +842,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,7 +890,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -896,13 +898,13 @@
         <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.2">
@@ -913,10 +915,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
@@ -924,13 +926,13 @@
         <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -941,10 +943,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="272" x14ac:dyDescent="0.2">
@@ -955,10 +957,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
@@ -969,10 +971,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -983,10 +985,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -997,10 +999,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -1011,10 +1013,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -1025,10 +1027,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.2">
@@ -1039,13 +1041,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
@@ -1053,10 +1055,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1083,10 +1085,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -1094,13 +1096,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1111,10 +1113,10 @@
         <v>20</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
@@ -1128,7 +1130,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
@@ -1139,7 +1141,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>53</v>
@@ -1156,7 +1158,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
@@ -1170,7 +1172,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
@@ -1181,10 +1183,10 @@
         <v>15</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -1195,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>